<commit_message>
first plot round done
</commit_message>
<xml_diff>
--- a/Data/MinimumWage_EuropeanUnion.xlsx
+++ b/Data/MinimumWage_EuropeanUnion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\susan\Documents\CodeProjects\00_OwnProjects\StateOfPostGradLiving\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49F63EA-1545-4AFA-AB03-99EAF0EB1153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1277DE9-40EF-41CE-B398-4956FC3F112F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EE747987-661C-458D-826F-6ADF49BD9E65}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Country</t>
   </si>
   <si>
-    <t>LastChecked</t>
-  </si>
-  <si>
     <t>Austria</t>
   </si>
   <si>
@@ -131,15 +128,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Varies</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>No statutory</t>
-  </si>
-  <si>
     <t>Wages set by collective agreements</t>
   </si>
   <si>
@@ -225,13 +213,19 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.sepe.es/HomeSepe/que-es-el-sepe/comunicacion-institucional/noticias/detalle-noticia?folder=/SEPE/2025/Febrero/&amp;detail=boe-publica-smi-2025-se-establece-1184-euros </t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Salaries/helsinki-finland-cleaner-salary-SRCH_IL.0,16_IM1005_KO17,24.htm</t>
+  </si>
+  <si>
+    <t>https://www.cxcglobal.com/global-hiring-guide/italy/payroll-and-benefits-in-italy/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +263,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -291,7 +293,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -312,6 +314,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -647,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5665E000-43D6-446C-BE43-FAA7016B3FFD}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,52 +663,45 @@
     <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5546875" customWidth="1"/>
     <col min="5" max="5" width="39.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>1700</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1">
+        <v>1418.95</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="1">
-        <v>20250821</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:10" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>2070</v>
@@ -715,15 +711,12 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="1">
-        <v>20250821</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="69" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>551</v>
@@ -733,13 +726,12 @@
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="41.4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>970</v>
@@ -749,13 +741,12 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>1000</v>
@@ -765,13 +756,12 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>850</v>
@@ -781,13 +771,12 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>886</v>
@@ -797,29 +786,29 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1859</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1236</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2300</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>1801.8</v>
@@ -829,13 +818,12 @@
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="41.4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>2222</v>
@@ -845,13 +833,12 @@
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>880</v>
@@ -861,13 +848,12 @@
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="41.4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>734.26</v>
@@ -877,13 +863,12 @@
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
         <v>2.282</v>
@@ -893,29 +878,29 @@
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C15" s="1">
+        <v>859.02</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" ht="69" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="B16" s="1">
         <v>740</v>
@@ -925,13 +910,13 @@
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" ht="41.4" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>1038</v>
@@ -941,13 +926,12 @@
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" ht="41.4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>2703.74</v>
@@ -957,13 +941,12 @@
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
         <v>961</v>
@@ -973,13 +956,12 @@
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>2505.6</v>
@@ -989,13 +971,12 @@
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="5">
         <v>1096.95</v>
@@ -1005,13 +986,12 @@
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" ht="207" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1">
         <v>870</v>
@@ -1021,13 +1001,12 @@
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" ht="69" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>801.55</v>
@@ -1037,13 +1016,12 @@
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>816</v>
@@ -1053,13 +1031,12 @@
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>1277.72</v>
@@ -1069,13 +1046,12 @@
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="6">
         <v>1184</v>
@@ -1085,13 +1061,12 @@
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1">
         <v>2090.91</v>
@@ -1100,20 +1075,18 @@
         <v>1507.36</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>